<commit_message>
updated code after meeting
</commit_message>
<xml_diff>
--- a/public/files/actualstock.xlsx
+++ b/public/files/actualstock.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sanjay\Projects\dmt\public\files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB913C2-4E50-433A-81AC-8994857D933F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="80" windowWidth="19140" windowHeight="7340"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>id</t>
   </si>
@@ -27,20 +33,11 @@
     <t>Actual 
 Stock</t>
   </si>
-  <si>
-    <t>date</t>
-  </si>
-  <si>
-    <t>month</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -101,7 +98,7 @@
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -113,6 +110,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -161,7 +161,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -194,9 +194,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -229,6 +246,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -404,20 +438,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD19"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.36328125" customWidth="1"/>
-    <col min="3" max="3" width="14.54296875" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,17 +461,8 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -447,17 +472,8 @@
       <c r="C2" s="3">
         <v>112193</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>6</v>
-      </c>
-      <c r="F2">
-        <v>2023</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -466,15 +482,6 @@
       </c>
       <c r="C3" s="3">
         <v>167320</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-      <c r="F3">
-        <v>2023</v>
       </c>
     </row>
   </sheetData>
@@ -483,24 +490,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>